<commit_message>
form centerd assignment on 0ct15
</commit_message>
<xml_diff>
--- a/assignment_result.xlsx
+++ b/assignment_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8535" windowHeight="6120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HTML" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="103">
   <si>
     <t>Anusha178</t>
   </si>
@@ -301,6 +301,39 @@
   </si>
   <si>
     <t>completed but &lt;article&gt; is missing</t>
+  </si>
+  <si>
+    <t>border of form is missing, pay attention to indentation</t>
+  </si>
+  <si>
+    <t>border of form is missing</t>
+  </si>
+  <si>
+    <t>doctype missing, put the files inside folders: template and styles,indentation is missing, where is the link to add external css? Wrong css</t>
+  </si>
+  <si>
+    <t>relative paths must be used, but still completed</t>
+  </si>
+  <si>
+    <t>completed but want to see it in action</t>
+  </si>
+  <si>
+    <t>indentation is missing, want to see it in action since relative path is missing</t>
+  </si>
+  <si>
+    <t>incomplete, where is the html file?</t>
+  </si>
+  <si>
+    <t>pay attention to indentation, border for the form is missing</t>
+  </si>
+  <si>
+    <t>completed but minor error, syntax for border is: border: 2px solid #bb3800; (&lt;dimension&gt; &lt;type&gt; &lt;color&gt;)</t>
+  </si>
+  <si>
+    <t>saikiran09</t>
+  </si>
+  <si>
+    <t>border of form is missing but everything else is good</t>
   </si>
 </sst>
 </file>
@@ -640,9 +673,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B46" sqref="B46"/>
+      <selection pane="topRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,17 +1329,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE40"/>
+  <dimension ref="A1:AE41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B42" sqref="B42"/>
+      <selection pane="topRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" customWidth="1"/>
+    <col min="2" max="2" width="124.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1410,16 +1443,25 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="5" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -1430,40 +1472,64 @@
       <c r="A6" t="s">
         <v>68</v>
       </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="8" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="B8" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>62</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1471,134 +1537,196 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>76</v>
+    <row r="15" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B19" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B24" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="B25" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B26" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B33" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="B34" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B36" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="B37" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+    <row r="39" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="40" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>58</v>
+      </c>
+      <c r="B41" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>